<commit_message>
Create ClassDiagram and databaseDiagram
</commit_message>
<xml_diff>
--- a/Baza.xlsx
+++ b/Baza.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sg0226566\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sg0226566\Desktop\Drab\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G16" sqref="G16:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,39 +503,33 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="17" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" s="1"/>
@@ -543,7 +537,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>